<commit_message>
correct some spelling mistakes (from meeting with Tara)
</commit_message>
<xml_diff>
--- a/Tests/Testübersicht mit Anzahl.xlsx
+++ b/Tests/Testübersicht mit Anzahl.xlsx
@@ -156,9 +156,6 @@
     <t>getallwitnesses/fromtradition/{tradId}</t>
   </si>
   <si>
-    <t>getallrealtionships/{tradId}</t>
-  </si>
-  <si>
     <t>gettradition/withid/{tradId}</t>
   </si>
   <si>
@@ -228,12 +225,6 @@
     <t>createuser</t>
   </si>
   <si>
-    <t>getuser/wihtid/{userId}</t>
-  </si>
-  <si>
-    <t>deleteuser/wihtid/{userId}</t>
-  </si>
-  <si>
     <t>gettraditions/ofuser/{userId}</t>
   </si>
   <si>
@@ -253,6 +244,15 @@
   </si>
   <si>
     <t>reorientStemma</t>
+  </si>
+  <si>
+    <t>deleteuser/withid/{userId}</t>
+  </si>
+  <si>
+    <t>getuser/withid/{userId}</t>
+  </si>
+  <si>
+    <t>getallrelationships/{tradId}</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -906,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -920,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -934,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -962,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="7" customFormat="1">
@@ -981,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>6</v>
@@ -995,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -1010,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>9</v>
@@ -1025,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
@@ -1040,7 +1040,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -1068,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -1082,7 +1082,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1110,7 +1110,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1129,10 +1129,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1146,7 +1146,7 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1187,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1201,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
@@ -1229,7 +1229,7 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
@@ -1259,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -1287,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -1320,10 +1320,10 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1334,7 +1334,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
@@ -1348,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
         <v>36</v>
@@ -1362,10 +1362,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D42" s="9">
         <v>5</v>

</xml_diff>